<commit_message>
Updated Configs file for the new enrty Demographic Data Validity of a TSP
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Configurations_Consolidated List_Updated_12Oct18_CV.xlsx
+++ b/requirements/MOSIP_Configurations_Consolidated List_Updated_12Oct18_CV.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1A89B235-0E7A-4386-BF65-455FAB65AC7E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7065" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7065" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kernel" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="266">
   <si>
     <r>
       <t xml:space="preserve">Configurations: </t>
@@ -984,15 +985,6 @@
     <t>Setup PDF template for Full e-KYC</t>
   </si>
   <si>
-    <t>Setup time zone for a country/state</t>
-  </si>
-  <si>
-    <t>UTC</t>
-  </si>
-  <si>
-    <t>UTC+1, UTC+5.30</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Configurations: </t>
     </r>
@@ -1054,12 +1046,15 @@
   <si>
     <t>Others to be added</t>
   </si>
+  <si>
+    <t>Setup the Demographic data validity for a TSP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2326,13 +2321,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2366,6 +2354,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2617,7 +2612,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="36"/>
       <tableStyleElement type="headerRow" dxfId="35"/>
     </tableStyle>
@@ -2634,60 +2629,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:F9" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="B2:F9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B2:F9" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="B2:F9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="2" name="Configuration Feature" dataDxfId="32"/>
-    <tableColumn id="1" name="Type of Config" dataDxfId="31"/>
-    <tableColumn id="3" name="Default Value" dataDxfId="30"/>
-    <tableColumn id="4" name="Other Values" dataDxfId="29"/>
-    <tableColumn id="5" name="Mindtree Comments" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Configuration Feature" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Type of Config" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Default Value" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Other Values" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Mindtree Comments" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A2:G27" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowBorderDxfId="24" tableBorderDxfId="25" totalsRowBorderDxfId="23">
-  <autoFilter ref="A2:G27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table22" displayName="Table22" ref="A2:G27" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+  <autoFilter ref="A2:G27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="S.No" dataDxfId="22"/>
-    <tableColumn id="2" name="Configuration Feature" dataDxfId="21"/>
-    <tableColumn id="3" name="Type of Config" dataDxfId="20"/>
-    <tableColumn id="4" name="Default Value" dataDxfId="19"/>
-    <tableColumn id="5" name="All Values" dataDxfId="18"/>
-    <tableColumn id="7" name="Mindtree Comments" dataDxfId="17"/>
-    <tableColumn id="6" name="Customer Comments" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="S.No" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Configuration Feature" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type of Config" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Default Value" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="All Values" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Mindtree Comments" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Customer Comments" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table224" displayName="Table224" ref="A2:E41" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A2:E41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table224" displayName="Table224" ref="A2:E41" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A2:E41" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="S.No" dataDxfId="13"/>
-    <tableColumn id="2" name="Configuration Feature" dataDxfId="12"/>
-    <tableColumn id="4" name="Type of Config" dataDxfId="11"/>
-    <tableColumn id="5" name="Default Value" dataDxfId="10"/>
-    <tableColumn id="6" name="Other Values" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="S.No" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Configuration Feature" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Type of Config" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Default Value" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Other Values" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table2245" displayName="Table2245" ref="A2:G35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:G35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table2245" displayName="Table2245" ref="A2:G35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A2:G35" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="S.No" dataDxfId="6"/>
-    <tableColumn id="2" name="Configuration Feature" dataDxfId="5"/>
-    <tableColumn id="4" name="Type of Config" dataDxfId="4"/>
-    <tableColumn id="5" name="Default Value" dataDxfId="3"/>
-    <tableColumn id="6" name="Other Values" dataDxfId="2"/>
-    <tableColumn id="3" name="Mindtree Comments" dataDxfId="1"/>
-    <tableColumn id="7" name="Customer Comments" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="S.No" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Configuration Feature" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Type of Config" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Default Value" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Other Values" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Mindtree Comments" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Customer Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2955,17 +2950,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="69" style="31" customWidth="1"/>
@@ -2977,7 +2972,7 @@
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
@@ -2989,7 +2984,7 @@
       <c r="G1" s="70"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
@@ -3013,7 +3008,7 @@
       </c>
       <c r="H2" s="31"/>
     </row>
-    <row r="3" spans="1:26" s="29" customFormat="1">
+    <row r="3" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -3049,7 +3044,7 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26" s="29" customFormat="1">
+    <row r="4" spans="1:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -3087,7 +3082,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" s="29" customFormat="1" ht="30">
+    <row r="5" spans="1:26" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>3</v>
       </c>
@@ -3125,7 +3120,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
     </row>
-    <row r="6" spans="1:26" s="29" customFormat="1" ht="30">
+    <row r="6" spans="1:26" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -3163,7 +3158,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:26" s="29" customFormat="1" ht="90">
+    <row r="7" spans="1:26" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>5</v>
       </c>
@@ -3201,7 +3196,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26" s="29" customFormat="1" ht="90">
+    <row r="8" spans="1:26" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -3239,7 +3234,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26" s="29" customFormat="1" ht="90">
+    <row r="9" spans="1:26" s="29" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -3277,7 +3272,7 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -3295,7 +3290,7 @@
       <c r="G10" s="37"/>
       <c r="H10" s="31"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
         <v>9</v>
       </c>
@@ -3313,7 +3308,7 @@
       <c r="G11" s="37"/>
       <c r="H11" s="31"/>
     </row>
-    <row r="12" spans="1:26" ht="90">
+    <row r="12" spans="1:26" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -3333,7 +3328,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="31"/>
     </row>
-    <row r="13" spans="1:26" ht="90">
+    <row r="13" spans="1:26" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>11</v>
       </c>
@@ -3351,7 +3346,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="31"/>
     </row>
-    <row r="14" spans="1:26" ht="90">
+    <row r="14" spans="1:26" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -3370,7 +3365,7 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:26" ht="30">
+    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <v>13</v>
       </c>
@@ -3389,7 +3384,7 @@
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -3406,7 +3401,7 @@
       </c>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7" ht="45">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="28">
         <v>15</v>
       </c>
@@ -3425,7 +3420,7 @@
       </c>
       <c r="G17" s="45"/>
     </row>
-    <row r="18" spans="1:7" ht="90">
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -3442,7 +3437,7 @@
       </c>
       <c r="G18" s="34"/>
     </row>
-    <row r="19" spans="1:7" ht="45">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="28">
         <v>17</v>
       </c>
@@ -3459,7 +3454,7 @@
       </c>
       <c r="G19" s="34"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="34"/>
       <c r="C20" s="37"/>
@@ -3481,7 +3476,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3489,7 +3484,7 @@
       <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="72" style="1" customWidth="1"/>
@@ -3500,7 +3495,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
         <v>37</v>
       </c>
@@ -3511,7 +3506,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="72"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
@@ -3534,7 +3529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="3" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -3555,7 +3550,7 @@
       </c>
       <c r="G3" s="40"/>
     </row>
-    <row r="4" spans="1:7" s="16" customFormat="1" ht="90">
+    <row r="4" spans="1:7" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -3574,7 +3569,7 @@
       </c>
       <c r="G4" s="40"/>
     </row>
-    <row r="5" spans="1:7" s="16" customFormat="1">
+    <row r="5" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -3595,7 +3590,7 @@
       </c>
       <c r="G5" s="40"/>
     </row>
-    <row r="6" spans="1:7" s="16" customFormat="1">
+    <row r="6" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -3616,7 +3611,7 @@
       </c>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="1:7" s="16" customFormat="1">
+    <row r="7" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -3637,7 +3632,7 @@
       </c>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="1:7" s="16" customFormat="1">
+    <row r="8" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -3658,7 +3653,7 @@
       </c>
       <c r="G8" s="40"/>
     </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" ht="120">
+    <row r="9" spans="1:7" s="16" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -3677,7 +3672,7 @@
       </c>
       <c r="G9" s="40"/>
     </row>
-    <row r="10" spans="1:7" s="16" customFormat="1">
+    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -3694,7 +3689,7 @@
       </c>
       <c r="G10" s="40"/>
     </row>
-    <row r="11" spans="1:7" s="16" customFormat="1">
+    <row r="11" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -3711,7 +3706,7 @@
       </c>
       <c r="G11" s="40"/>
     </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="12" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -3728,7 +3723,7 @@
       </c>
       <c r="G12" s="40"/>
     </row>
-    <row r="13" spans="1:7" s="16" customFormat="1">
+    <row r="13" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -3745,7 +3740,7 @@
       </c>
       <c r="G13" s="40"/>
     </row>
-    <row r="14" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="14" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -3762,7 +3757,7 @@
       </c>
       <c r="G14" s="40"/>
     </row>
-    <row r="15" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="15" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -3779,7 +3774,7 @@
       </c>
       <c r="G15" s="40"/>
     </row>
-    <row r="16" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="16" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -3796,7 +3791,7 @@
       </c>
       <c r="G16" s="40"/>
     </row>
-    <row r="17" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="17" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -3813,7 +3808,7 @@
       </c>
       <c r="G17" s="40"/>
     </row>
-    <row r="18" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="18" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -3830,7 +3825,7 @@
       </c>
       <c r="G18" s="40"/>
     </row>
-    <row r="19" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="19" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -3851,7 +3846,7 @@
       </c>
       <c r="G19" s="40"/>
     </row>
-    <row r="20" spans="1:7" s="16" customFormat="1">
+    <row r="20" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -3868,7 +3863,7 @@
       </c>
       <c r="G20" s="40"/>
     </row>
-    <row r="21" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="21" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -3885,7 +3880,7 @@
       </c>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="1:7" s="16" customFormat="1" ht="30">
+    <row r="22" spans="1:7" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -3904,7 +3899,7 @@
       </c>
       <c r="G22" s="40"/>
     </row>
-    <row r="23" spans="1:7" s="16" customFormat="1">
+    <row r="23" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -3923,7 +3918,7 @@
       </c>
       <c r="G23" s="40"/>
     </row>
-    <row r="24" spans="1:7" ht="27" customHeight="1">
+    <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -3940,7 +3935,7 @@
       </c>
       <c r="G24" s="40"/>
     </row>
-    <row r="25" spans="1:7" ht="45">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -3959,7 +3954,7 @@
       </c>
       <c r="G25" s="40"/>
     </row>
-    <row r="26" spans="1:7" ht="30">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -3976,7 +3971,7 @@
       </c>
       <c r="G26" s="40"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>25</v>
       </c>
@@ -3993,7 +3988,7 @@
       <c r="F27" s="65"/>
       <c r="G27" s="65"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>81</v>
       </c>
@@ -4012,7 +4007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4020,7 +4015,7 @@
       <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="14" customWidth="1"/>
     <col min="2" max="2" width="62" style="7" customWidth="1"/>
@@ -4030,7 +4025,7 @@
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
         <v>82</v>
       </c>
@@ -4041,7 +4036,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="73"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4064,7 +4059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -4083,7 +4078,7 @@
       </c>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="90">
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -4104,7 +4099,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -4125,7 +4120,7 @@
       </c>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" ht="135">
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -4142,7 +4137,7 @@
       </c>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" ht="75">
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -4159,7 +4154,7 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="90">
+    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -4180,7 +4175,7 @@
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -4201,7 +4196,7 @@
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -4222,7 +4217,7 @@
       </c>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -4243,7 +4238,7 @@
       </c>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -4264,7 +4259,7 @@
       </c>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -4285,7 +4280,7 @@
       </c>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" ht="45">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -4306,7 +4301,7 @@
       </c>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="60">
+    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -4327,7 +4322,7 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -4346,7 +4341,7 @@
       </c>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -4365,7 +4360,7 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -4382,7 +4377,7 @@
       </c>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -4399,7 +4394,7 @@
       </c>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -4416,7 +4411,7 @@
       </c>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -4433,7 +4428,7 @@
       </c>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -4450,7 +4445,7 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -4467,7 +4462,7 @@
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -4484,7 +4479,7 @@
       </c>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -4501,7 +4496,7 @@
       </c>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -4518,7 +4513,7 @@
       </c>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -4535,7 +4530,7 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -4552,7 +4547,7 @@
       </c>
       <c r="G28" s="12"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -4569,7 +4564,7 @@
       </c>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>28</v>
       </c>
@@ -4586,7 +4581,7 @@
       </c>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>29</v>
       </c>
@@ -4603,7 +4598,7 @@
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:7" ht="150">
+    <row r="32" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -4620,7 +4615,7 @@
       </c>
       <c r="G32" s="9"/>
     </row>
-    <row r="33" spans="1:7" ht="105">
+    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>31</v>
       </c>
@@ -4639,7 +4634,7 @@
       </c>
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>32</v>
       </c>
@@ -4660,7 +4655,7 @@
       </c>
       <c r="G34" s="9"/>
     </row>
-    <row r="35" spans="1:7" ht="30">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>33</v>
       </c>
@@ -4679,7 +4674,7 @@
       </c>
       <c r="G35" s="9"/>
     </row>
-    <row r="36" spans="1:7" ht="30">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34</v>
       </c>
@@ -4698,7 +4693,7 @@
       </c>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="1:7" ht="45">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>35</v>
       </c>
@@ -4719,7 +4714,7 @@
       </c>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="1:7" ht="30">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>36</v>
       </c>
@@ -4740,7 +4735,7 @@
       </c>
       <c r="G38" s="9"/>
     </row>
-    <row r="39" spans="1:7" ht="30">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>37</v>
       </c>
@@ -4761,7 +4756,7 @@
       </c>
       <c r="G39" s="9"/>
     </row>
-    <row r="40" spans="1:7" ht="75">
+    <row r="40" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>38</v>
       </c>
@@ -4778,7 +4773,7 @@
       </c>
       <c r="G40" s="9"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>39</v>
       </c>
@@ -4795,7 +4790,7 @@
       </c>
       <c r="G41" s="9"/>
     </row>
-    <row r="42" spans="1:7" ht="60">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="38">
         <v>40</v>
       </c>
@@ -4816,7 +4811,7 @@
       </c>
       <c r="G42" s="9"/>
     </row>
-    <row r="43" spans="1:7" ht="60">
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="38">
         <v>41</v>
       </c>
@@ -4837,7 +4832,7 @@
       </c>
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:7" s="1" customFormat="1" ht="30">
+    <row r="44" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>42</v>
       </c>
@@ -4867,17 +4862,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomRight" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="14"/>
     <col min="2" max="2" width="62" style="7" customWidth="1"/>
@@ -4887,7 +4882,7 @@
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
         <v>156</v>
       </c>
@@ -4898,7 +4893,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="73"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4921,7 +4916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="38">
         <v>1</v>
       </c>
@@ -4940,7 +4935,7 @@
       </c>
       <c r="G3" s="55"/>
     </row>
-    <row r="4" spans="1:7" ht="45">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="38">
         <v>2</v>
       </c>
@@ -4961,7 +4956,7 @@
       </c>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:7" ht="75">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
         <v>3</v>
       </c>
@@ -4978,7 +4973,7 @@
       </c>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="38">
         <v>4</v>
       </c>
@@ -4999,7 +4994,7 @@
       </c>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="38">
         <v>5</v>
       </c>
@@ -5020,7 +5015,7 @@
       </c>
       <c r="G7" s="22"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="38">
         <v>6</v>
       </c>
@@ -5041,7 +5036,7 @@
       </c>
       <c r="G8" s="22"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="38">
         <v>7</v>
       </c>
@@ -5062,7 +5057,7 @@
       </c>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="38">
         <v>8</v>
       </c>
@@ -5083,7 +5078,7 @@
       </c>
       <c r="G10" s="22"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>9</v>
       </c>
@@ -5104,7 +5099,7 @@
       </c>
       <c r="G11" s="22"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>10</v>
       </c>
@@ -5125,7 +5120,7 @@
       </c>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="38">
         <v>11</v>
       </c>
@@ -5146,7 +5141,7 @@
       </c>
       <c r="G13" s="22"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
         <v>12</v>
       </c>
@@ -5167,7 +5162,7 @@
       </c>
       <c r="G14" s="22"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="38">
         <v>13</v>
       </c>
@@ -5184,7 +5179,7 @@
       </c>
       <c r="G15" s="22"/>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="38">
         <v>14</v>
       </c>
@@ -5205,7 +5200,7 @@
       </c>
       <c r="G16" s="22"/>
     </row>
-    <row r="17" spans="1:7" ht="30">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="38">
         <v>15</v>
       </c>
@@ -5226,7 +5221,7 @@
       </c>
       <c r="G17" s="22"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="38">
         <v>16</v>
       </c>
@@ -5247,7 +5242,7 @@
       </c>
       <c r="G18" s="22"/>
     </row>
-    <row r="19" spans="1:7" ht="30">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="38">
         <v>17</v>
       </c>
@@ -5268,7 +5263,7 @@
       </c>
       <c r="G19" s="22"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="38">
         <v>18</v>
       </c>
@@ -5285,7 +5280,7 @@
       </c>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="38">
         <v>19</v>
       </c>
@@ -5304,7 +5299,7 @@
       </c>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="38">
         <v>20</v>
       </c>
@@ -5321,7 +5316,7 @@
       </c>
       <c r="G22" s="22"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>21</v>
       </c>
@@ -5338,7 +5333,7 @@
       </c>
       <c r="G23" s="22"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="38">
         <v>22</v>
       </c>
@@ -5357,7 +5352,7 @@
       </c>
       <c r="G24" s="22"/>
     </row>
-    <row r="25" spans="1:7" ht="45">
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
         <v>23</v>
       </c>
@@ -5376,7 +5371,7 @@
       </c>
       <c r="G25" s="22"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
         <v>24</v>
       </c>
@@ -5395,7 +5390,7 @@
       </c>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>25</v>
       </c>
@@ -5414,7 +5409,7 @@
       </c>
       <c r="G27" s="22"/>
     </row>
-    <row r="28" spans="1:7" ht="30">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="38">
         <v>26</v>
       </c>
@@ -5429,7 +5424,7 @@
       </c>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:7" ht="30">
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="38">
         <v>27</v>
       </c>
@@ -5444,7 +5439,7 @@
       </c>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:7" ht="30">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="38">
         <v>28</v>
       </c>
@@ -5459,7 +5454,7 @@
       </c>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="1:7" ht="30">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="38">
         <v>29</v>
       </c>
@@ -5474,7 +5469,7 @@
       </c>
       <c r="G31" s="22"/>
     </row>
-    <row r="32" spans="1:7" ht="30">
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
         <v>30</v>
       </c>
@@ -5489,7 +5484,7 @@
       </c>
       <c r="G32" s="22"/>
     </row>
-    <row r="33" spans="1:7" ht="30">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
         <v>31</v>
       </c>
@@ -5504,7 +5499,7 @@
       </c>
       <c r="G33" s="22"/>
     </row>
-    <row r="34" spans="1:7" ht="30">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="38">
         <v>32</v>
       </c>
@@ -5519,7 +5514,7 @@
       </c>
       <c r="G34" s="22"/>
     </row>
-    <row r="35" spans="1:7" ht="30">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
         <v>33</v>
       </c>
@@ -5547,17 +5542,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="72" style="7" customWidth="1"/>
@@ -5569,7 +5564,7 @@
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
         <v>207</v>
       </c>
@@ -5580,7 +5575,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="73"/>
     </row>
-    <row r="2" spans="1:7" s="32" customFormat="1" ht="12.75">
+    <row r="2" spans="1:7" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
@@ -5603,7 +5598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="225">
+    <row r="3" spans="1:7" ht="240" x14ac:dyDescent="0.25">
       <c r="A3" s="33">
         <v>1</v>
       </c>
@@ -5624,7 +5619,7 @@
       </c>
       <c r="G3" s="34"/>
     </row>
-    <row r="4" spans="1:7" ht="45">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="33">
         <v>2</v>
       </c>
@@ -5645,7 +5640,7 @@
       </c>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
         <v>3</v>
       </c>
@@ -5666,7 +5661,7 @@
       </c>
       <c r="G5" s="37"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
         <v>4</v>
       </c>
@@ -5685,7 +5680,7 @@
       </c>
       <c r="G6" s="37"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>5</v>
       </c>
@@ -5704,7 +5699,7 @@
       </c>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>6</v>
       </c>
@@ -5725,7 +5720,7 @@
       </c>
       <c r="G8" s="37"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
         <v>7</v>
       </c>
@@ -5744,7 +5739,7 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
         <v>8</v>
       </c>
@@ -5763,7 +5758,7 @@
       </c>
       <c r="G10" s="37"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
         <v>9</v>
       </c>
@@ -5780,7 +5775,7 @@
       </c>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
         <v>10</v>
       </c>
@@ -5797,7 +5792,7 @@
       </c>
       <c r="G12" s="37"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
         <v>11</v>
       </c>
@@ -5814,7 +5809,7 @@
       </c>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
         <v>12</v>
       </c>
@@ -5831,7 +5826,7 @@
       </c>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
         <v>13</v>
       </c>
@@ -5852,7 +5847,7 @@
       </c>
       <c r="G15" s="34"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
         <v>14</v>
       </c>
@@ -5873,7 +5868,7 @@
       </c>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
         <v>15</v>
       </c>
@@ -5894,7 +5889,7 @@
       </c>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
         <v>16</v>
       </c>
@@ -5915,7 +5910,7 @@
       </c>
       <c r="G18" s="37"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
         <v>17</v>
       </c>
@@ -5932,7 +5927,7 @@
       </c>
       <c r="G19" s="37"/>
     </row>
-    <row r="20" spans="1:7" ht="30">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
         <v>18</v>
       </c>
@@ -5949,7 +5944,7 @@
       </c>
       <c r="G20" s="37"/>
     </row>
-    <row r="21" spans="1:7" ht="30">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
         <v>19</v>
       </c>
@@ -5970,7 +5965,7 @@
       </c>
       <c r="G21" s="37"/>
     </row>
-    <row r="22" spans="1:7" ht="30">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
         <v>20</v>
       </c>
@@ -5991,7 +5986,7 @@
       </c>
       <c r="G22" s="37"/>
     </row>
-    <row r="23" spans="1:7" ht="30">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
         <v>21</v>
       </c>
@@ -6012,7 +6007,7 @@
       </c>
       <c r="G23" s="37"/>
     </row>
-    <row r="24" spans="1:7" ht="30">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
         <v>22</v>
       </c>
@@ -6033,7 +6028,7 @@
       </c>
       <c r="G24" s="37"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
         <v>23</v>
       </c>
@@ -6048,7 +6043,7 @@
       <c r="F25" s="34"/>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
         <v>24</v>
       </c>
@@ -6063,21 +6058,21 @@
       <c r="F26" s="34"/>
       <c r="G26" s="37"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
         <v>25</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="C27" s="36" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>251</v>
+        <v>27</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="37"/>
@@ -6092,14 +6087,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="76.5703125" style="7" customWidth="1"/>
@@ -6110,9 +6105,9 @@
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B1" s="72"/>
       <c r="C1" s="72"/>
@@ -6121,7 +6116,7 @@
       <c r="F1" s="72"/>
       <c r="G1" s="73"/>
     </row>
-    <row r="2" spans="1:7" s="32" customFormat="1" ht="12.75">
+    <row r="2" spans="1:7" s="32" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
@@ -6144,27 +6139,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="33">
         <v>1</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
       <c r="F3" s="37" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:7" ht="45">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="33">
         <v>2</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C4" s="36"/>
       <c r="D4" s="37"/>
@@ -6174,12 +6169,12 @@
       </c>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
         <v>3</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>9</v>
@@ -6191,35 +6186,35 @@
         <v>180</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G5" s="34"/>
     </row>
-    <row r="6" spans="1:7" ht="60">
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
         <v>4</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E6" s="34"/>
       <c r="F6" s="34" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>5</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="37"/>
@@ -6229,12 +6224,12 @@
       </c>
       <c r="G7" s="37"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>6</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="37"/>
@@ -6244,12 +6239,12 @@
       </c>
       <c r="G8" s="37"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
         <v>7</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="37"/>
@@ -6259,12 +6254,12 @@
       </c>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
         <v>8</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="37"/>
@@ -6274,12 +6269,12 @@
       </c>
       <c r="G10" s="37"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
         <v>9</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="37"/>
@@ -6289,12 +6284,12 @@
       </c>
       <c r="G11" s="37"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
         <v>10</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="37"/>
@@ -6312,15 +6307,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="CTDocLibrary" ma:contentTypeID="0x010100C5D5EC2DEF914E3897774E287F80A8FB00C54CAAC0C88AA446A5AFE942C68BA98B" ma:contentTypeVersion="8" ma:contentTypeDescription="My Content Type" ma:contentTypeScope="" ma:versionID="8509de5a9a506e3b9b1fe93a7c193cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="fd9ad297-cc8c-4afc-b828-e13c9647a5fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b380538c208c9f76b13ef3dbebc9c2d9" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6527,6 +6513,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6554,14 +6549,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3174CE2-5708-4158-93D0-CBBFFB333158}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E8A634F-74FC-499D-ABEA-0CA6D30F983F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6580,6 +6567,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3174CE2-5708-4158-93D0-CBBFFB333158}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50A5568B-AE5A-4E16-9E1F-F6758BCAE61C}">
   <ds:schemaRefs>

</xml_diff>